<commit_message>
updated new leagues division
</commit_message>
<xml_diff>
--- a/CHN.xlsx
+++ b/CHN.xlsx
@@ -518,340 +518,340 @@
     <t>Team against</t>
   </si>
   <si>
-    <t>Beijing Guoan,L L W W W D L D W W D L W W</t>
-  </si>
-  <si>
-    <t>Cangzhou,L D D L D L L W L D L L W L</t>
-  </si>
-  <si>
-    <t>Changchun Yatai,W D D D W L W W D W W W L W</t>
-  </si>
-  <si>
-    <t>Chongqing Liangjiang Athletic,L L D W L L L L W D L W L L</t>
-  </si>
-  <si>
-    <t>Dalian Pro,L L L W L L D L L W L L L L</t>
-  </si>
-  <si>
-    <t>Guangzhou City,D W W L D D D D L W W W L D</t>
-  </si>
-  <si>
-    <t>Guangzhou FC,D L W W D W W D W L W W W W</t>
-  </si>
-  <si>
-    <t>Hebei,D W W D L W L W W D D L W D</t>
-  </si>
-  <si>
-    <t>Henan Songshan Longmen,L D D L D W D D W L W L W D</t>
-  </si>
-  <si>
-    <t>Qingdao FC,W D L L W L L L L L L L L L</t>
-  </si>
-  <si>
-    <t>Shandong Taishan,W W D W D D W W L W W W W W</t>
-  </si>
-  <si>
-    <t>Shanghai Port,W W D D W D W D W L W W L W</t>
-  </si>
-  <si>
-    <t>Shanghai Shenhua,W W D D L W W D L D L W W L</t>
-  </si>
-  <si>
-    <t>Shenzhen,W D L W D W W D W W L L L W</t>
-  </si>
-  <si>
-    <t>Tianjin Jinmen Tiger,L D L L W D L L L L D W L L</t>
-  </si>
-  <si>
-    <t>Wuhan FC,D L D L L D D D D L D L W D</t>
-  </si>
-  <si>
-    <t>Beijing Guoan,1 1 2 2 2 0 0 1 1 2 0 1 2 4,(19)</t>
-  </si>
-  <si>
-    <t>Cangzhou,1 0 2 0 0 1 0 2 1 1 2 0 2 1,(13)</t>
-  </si>
-  <si>
-    <t>Changchun Yatai,2 0 0 0 1 1 2 4 2 2 2 3 1 3,(23)</t>
-  </si>
-  <si>
-    <t>Chongqing Liangjiang Athletic,0 1 2 3 0 1 0 1 4 1 0 1 1 1,(16)</t>
-  </si>
-  <si>
-    <t>Dalian Pro,1 0 0 1 0 2 1 0 0 3 0 2 1 1,(12)</t>
-  </si>
-  <si>
-    <t>Guangzhou City,2 3 1 2 0 0 1 3 0 4 1 2 1 1,(21)</t>
-  </si>
-  <si>
-    <t>Guangzhou FC,2 0 2 2 1 3 6 3 2 1 5 2 5 5,(39)</t>
-  </si>
-  <si>
-    <t>Hebei,1 1 1 1 1 2 0 1 2 0 0 0 1 1,(12)</t>
-  </si>
-  <si>
-    <t>Henan Songshan Longmen,1 0 1 2 1 2 1 0 2 0 1 0 1 1,(13)</t>
-  </si>
-  <si>
-    <t>Qingdao FC,2 0 0 0 1 0 0 0 1 2 0 0 0 0,(6)</t>
-  </si>
-  <si>
-    <t>Shandong Taishan,2 1 1 2 2 0 2 3 1 2 5 4 3 2,(30)</t>
-  </si>
-  <si>
-    <t>Shanghai Port,6 3 1 0 3 0 1 1 1 1 5 3 0 5,(30)</t>
-  </si>
-  <si>
-    <t>Shanghai Shenhua,2 3 1 1 0 3 3 0 0 0 1 4 1 2,(21)</t>
-  </si>
-  <si>
-    <t>Shenzhen,2 0 0 4 2 2 3 0 4 2 0 2 1 2,(24)</t>
-  </si>
-  <si>
-    <t>Tianjin Jinmen Tiger,1 0 0 0 2 0 1 1 1 1 1 3 0 0,(11)</t>
-  </si>
-  <si>
-    <t>Wuhan FC,1 1 0 0 1 0 1 0 2 1 1 0 2 1,(11)</t>
-  </si>
-  <si>
-    <t>Beijing Guoan,2 3 0 0 1 0 2 1 0 1 0 3 1 2,(16)</t>
-  </si>
-  <si>
-    <t>Cangzhou,2 0 2 2 0 2 2 0 2 1 5 2 1 2,(23)</t>
-  </si>
-  <si>
-    <t>Changchun Yatai,1 0 0 0 0 2 0 1 2 1 1 0 2 1,(11)</t>
-  </si>
-  <si>
-    <t>Chongqing Liangjiang Athletic,2 3 2 2 1 3 3 3 0 1 1 0 5 2,(28)</t>
-  </si>
-  <si>
-    <t>Dalian Pro,2 1 2 0 3 3 1 1 1 1 5 4 2 3,(29)</t>
-  </si>
-  <si>
-    <t>Guangzhou City,2 1 0 4 0 0 1 3 4 2 0 0 3 1,(21)</t>
-  </si>
-  <si>
-    <t>Guangzhou FC,2 1 0 0 1 1 0 3 1 2 2 0 1 0,(14)</t>
-  </si>
-  <si>
-    <t>Hebei,1 0 0 1 2 1 1 0 1 0 0 3 0 1,(11)</t>
-  </si>
-  <si>
-    <t>Henan Songshan Longmen,2 0 1 3 1 0 1 0 1 2 0 2 0 1,(14)</t>
-  </si>
-  <si>
-    <t>Qingdao FC,1 0 1 2 0 2 6 2 4 4 5 1 1 5,(34)</t>
-  </si>
-  <si>
-    <t>Shandong Taishan,0 0 1 0 2 0 0 1 2 0 0 2 1 1,(10)</t>
-  </si>
-  <si>
-    <t>Shanghai Port,1 1 1 0 0 0 0 1 0 2 0 0 1 0,(7)</t>
-  </si>
-  <si>
-    <t>Shanghai Shenhua,1 1 1 1 1 2 1 0 1 0 2 2 0 4,(17)</t>
-  </si>
-  <si>
-    <t>Shenzhen,1 0 2 2 2 1 0 0 1 1 1 4 2 1,(18)</t>
-  </si>
-  <si>
-    <t>Tianjin Jinmen Tiger,6 0 1 1 1 0 3 4 2 3 1 1 1 5,(29)</t>
-  </si>
-  <si>
-    <t>Wuhan FC,1 3 0 2 2 0 1 0 2 2 1 3 1 1,(19)</t>
-  </si>
-  <si>
-    <t>Beijing Guoan,3 4 2 2 3 0 2 2 1 3 0 4 3 6,(35)</t>
-  </si>
-  <si>
-    <t>Cangzhou,3 0 4 2 0 3 2 2 3 2 7 2 3 3,(36)</t>
-  </si>
-  <si>
-    <t>Changchun Yatai,3 0 0 0 1 3 2 5 4 3 3 3 3 4,(34)</t>
-  </si>
-  <si>
-    <t>Chongqing Liangjiang Athletic,2 4 4 5 1 4 3 4 4 2 1 1 6 3,(44)</t>
-  </si>
-  <si>
-    <t>Dalian Pro,3 1 2 1 3 5 2 1 1 4 5 6 3 4,(41)</t>
-  </si>
-  <si>
-    <t>Guangzhou City,4 4 1 6 0 0 2 6 4 6 1 2 4 2,(42)</t>
-  </si>
-  <si>
-    <t>Guangzhou FC,4 1 2 2 2 4 6 6 3 3 7 2 6 5,(53)</t>
-  </si>
-  <si>
-    <t>Hebei,2 1 1 2 3 3 1 1 3 0 0 3 1 2,(23)</t>
-  </si>
-  <si>
-    <t>Henan Songshan Longmen,3 0 2 5 2 2 2 0 3 2 1 2 1 2,(27)</t>
-  </si>
-  <si>
-    <t>Qingdao FC,3 0 1 2 1 2 6 2 5 6 5 1 1 5,(40)</t>
-  </si>
-  <si>
-    <t>Shandong Taishan,2 1 2 2 4 0 2 4 3 2 5 6 4 3,(40)</t>
-  </si>
-  <si>
-    <t>Shanghai Port,7 4 2 0 3 0 1 2 1 3 5 3 1 5,(37)</t>
-  </si>
-  <si>
-    <t>Shanghai Shenhua,3 4 2 2 1 5 4 0 1 0 3 6 1 6,(38)</t>
-  </si>
-  <si>
-    <t>Shenzhen,3 0 2 6 4 3 3 0 5 3 1 6 3 3,(42)</t>
-  </si>
-  <si>
-    <t>Tianjin Jinmen Tiger,7 0 1 1 3 0 4 5 3 4 2 4 1 5,(40)</t>
-  </si>
-  <si>
-    <t>Wuhan FC,2 4 0 2 3 0 2 0 4 3 2 3 3 2,(30)</t>
-  </si>
-  <si>
-    <t>Beijing Guoan,2-1 3-1 2-0 0-2 2-1 0-0 2-0 1-1 0-1 2-1 0-0 3-1 2-1 4-2</t>
-  </si>
-  <si>
-    <t>Cangzhou,2-1 0-0 2-2 0-2 0-0 2-1 0-2 2-0 2-1 1-1 5-2 0-2 2-1 2-1</t>
-  </si>
-  <si>
-    <t>Changchun Yatai,1-2 0-0 0-0 0-0 1-0 2-1 2-0 1-4 2-2 2-1 1-2 3-0 2-1 3-1</t>
-  </si>
-  <si>
-    <t>Chongqing Liangjiang Athletic,0-2 3-1 2-2 3-2 1-0 3-1 0-3 3-1 4-0 1-1 1-0 1-0 1-5 2-1</t>
-  </si>
-  <si>
-    <t>Dalian Pro,1-2 0-1 2-0 1-0 3-0 3-2 1-1 1-0 0-1 1-3 0-5 2-4 2-1 3-1</t>
-  </si>
-  <si>
-    <t>Guangzhou City,2-2 3-1 0-1 2-4 0-0 0-0 1-1 3-3 4-0 4-2 0-1 0-2 1-3 1-1</t>
-  </si>
-  <si>
-    <t>Guangzhou FC,2-2 1-0 2-0 0-2 1-1 3-1 0-6 3-3 2-1 2-1 5-2 2-0 1-5 5-0</t>
-  </si>
-  <si>
-    <t>Hebei,1-1 0-1 0-1 1-1 2-1 2-1 1-0 1-0 2-1 0-0 0-0 3-0 1-0 1-1</t>
-  </si>
-  <si>
-    <t>Henan Songshan Longmen,1-2 0-0 1-1 3-2 1-1 2-0 1-1 0-0 2-1 2-0 1-0 2-0 0-1 1-1</t>
-  </si>
-  <si>
-    <t>Qingdao FC,2-1 0-0 0-1 2-0 1-0 2-0 0-6 2-0 1-4 4-2 0-5 1-0 0-1 5-0</t>
-  </si>
-  <si>
-    <t>Shandong Taishan,0-2 1-0 1-1 2-0 2-2 0-0 0-2 3-1 2-1 2-0 0-5 4-2 1-3 2-1</t>
-  </si>
-  <si>
-    <t>Shanghai Port,1-6 3-1 1-1 0-0 3-0 0-0 1-0 1-1 1-0 2-1 0-5 3-0 1-0 5-0</t>
-  </si>
-  <si>
-    <t>Shanghai Shenhua,2-1 1-3 1-1 1-1 1-0 3-2 1-3 0-0 1-0 0-0 1-2 2-4 1-0 4-2</t>
-  </si>
-  <si>
-    <t>Shenzhen,1-2 0-0 2-0 2-4 2-2 2-1 0-3 0-0 1-4 2-1 0-1 4-2 2-1 2-1</t>
-  </si>
-  <si>
-    <t>Tianjin Jinmen Tiger,1-6 0-0 0-1 1-0 2-1 0-0 1-3 1-4 2-1 1-3 1-1 3-1 1-0 5-0</t>
-  </si>
-  <si>
-    <t>Wuhan FC,1-1 1-3 0-0 0-2 2-1 0-0 1-1 0-0 2-2 2-1 1-1 3-0 2-1 1-1</t>
-  </si>
-  <si>
-    <t>Beijing Guoan,-1 -2 2 2 1 0 -2 0 1 1 0 -2 1 2,(3)</t>
-  </si>
-  <si>
-    <t>Cangzhou,-1 0 0 -2 0 -1 -2 2 -1 0 -3 -2 1 -1,(-10)</t>
-  </si>
-  <si>
-    <t>Changchun Yatai,1 0 0 0 1 -1 2 3 0 1 1 3 -1 2,(12)</t>
-  </si>
-  <si>
-    <t>Chongqing Liangjiang Athletic,-2 -2 0 1 -1 -2 -3 -2 4 0 -1 1 -4 -1,(-12)</t>
-  </si>
-  <si>
-    <t>Dalian Pro,-1 -1 -2 1 -3 -1 0 -1 -1 2 -5 -2 -1 -2,(-17)</t>
-  </si>
-  <si>
-    <t>Guangzhou City,0 2 1 -2 0 0 0 0 -4 2 1 2 -2 0,(0)</t>
-  </si>
-  <si>
-    <t>Guangzhou FC,0 -1 2 2 0 2 6 0 1 -1 3 2 4 5,(25)</t>
-  </si>
-  <si>
-    <t>Hebei,0 1 1 0 -1 1 -1 1 1 0 0 -3 1 0,(1)</t>
-  </si>
-  <si>
-    <t>Henan Songshan Longmen,-1 0 0 -1 0 2 0 0 1 -2 1 -2 1 0,(-1)</t>
-  </si>
-  <si>
-    <t>Qingdao FC,1 0 -1 -2 1 -2 -6 -2 -3 -2 -5 -1 -1 -5,(-28)</t>
-  </si>
-  <si>
-    <t>Shandong Taishan,2 1 0 2 0 0 2 2 -1 2 5 2 2 1,(20)</t>
-  </si>
-  <si>
-    <t>Shanghai Port,5 2 0 0 3 0 1 0 1 -1 5 3 -1 5,(23)</t>
-  </si>
-  <si>
-    <t>Shanghai Shenhua,1 2 0 0 -1 1 2 0 -1 0 -1 2 1 -2,(4)</t>
-  </si>
-  <si>
-    <t>Shenzhen,1 0 -2 2 0 1 3 0 3 1 -1 -2 -1 1,(6)</t>
-  </si>
-  <si>
-    <t>Tianjin Jinmen Tiger,-5 0 -1 -1 1 0 -2 -3 -1 -2 0 2 -1 -5,(-18)</t>
-  </si>
-  <si>
-    <t>Wuhan FC,0 -2 0 -2 -1 0 0 0 0 -1 0 -3 1 0,(-8)</t>
-  </si>
-  <si>
-    <t>Beijing Guoan,Shanghai Shenhua(8) Shanghai Port(4) Dalian Pro(15) Wuhan FC(12) Hebei(7) Tianjin Jinmen Tiger(14) Changchun Yatai(3) Shanghai Port(4) Dalian Pro(15) Wuhan FC(12) Hebei(7) Tianjin Jinmen Tiger(14) Changchun Yatai(3) Shanghai Shenhua(8)</t>
-  </si>
-  <si>
-    <t>Cangzhou,Qingdao FC(16) Henan Songshan Longmen(10) Chongqing Liangjiang Athletic(11) Guangzhou FC(2) Guangzhou City(9) Shenzhen(6) Shandong Taishan(1) Qingdao FC(16) Henan Songshan Longmen(10) Chongqing Liangjiang Athletic(11) Guangzhou FC(2) Guangzhou City(9) Shenzhen(6) Shandong Taishan(1)</t>
-  </si>
-  <si>
-    <t>Changchun Yatai,Dalian Pro(15) Tianjin Jinmen Tiger(14) Wuhan FC(12) Shanghai Port(4) Shanghai Shenhua(8) Hebei(7) Beijing Guoan(5) Tianjin Jinmen Tiger(14) Wuhan FC(12) Shanghai Port(4) Shanghai Shenhua(8) Hebei(7) Beijing Guoan(5) Dalian Pro(15)</t>
-  </si>
-  <si>
-    <t>Chongqing Liangjiang Athletic,Shandong Taishan(1) Guangzhou City(9) Cangzhou(13) Henan Songshan Longmen(10) Qingdao FC(16) Guangzhou FC(2) Shenzhen(6) Shandong Taishan(1) Guangzhou City(9) Cangzhou(13) Henan Songshan Longmen(10) Qingdao FC(16) Guangzhou FC(2) Shenzhen(6)</t>
-  </si>
-  <si>
-    <t>Dalian Pro,Changchun Yatai(3) Hebei(7) Beijing Guoan(5) Tianjin Jinmen Tiger(14) Shanghai Port(4) Shanghai Shenhua(8) Wuhan FC(12) Hebei(7) Beijing Guoan(5) Tianjin Jinmen Tiger(14) Shanghai Port(4) Shanghai Shenhua(8) Wuhan FC(12) Changchun Yatai(3)</t>
-  </si>
-  <si>
-    <t>Guangzhou City,Guangzhou FC(2) Chongqing Liangjiang Athletic(11) Qingdao FC(16) Shenzhen(6) Cangzhou(13) Shandong Taishan(1) Henan Songshan Longmen(10) Guangzhou FC(2) Chongqing Liangjiang Athletic(11) Qingdao FC(16) Shenzhen(6) Cangzhou(13) Shandong Taishan(1) Henan Songshan Longmen(10)</t>
-  </si>
-  <si>
-    <t>Guangzhou FC,Guangzhou City(9) Shandong Taishan(1) Shenzhen(6) Cangzhou(13) Henan Songshan Longmen(10) Chongqing Liangjiang Athletic(11) Qingdao FC(16) Guangzhou City(9) Shandong Taishan(1) Shenzhen(6) Cangzhou(13) Henan Songshan Longmen(10) Chongqing Liangjiang Athletic(11) Qingdao FC(16)</t>
-  </si>
-  <si>
-    <t>Hebei,Wuhan FC(12) Dalian Pro(15) Tianjin Jinmen Tiger(14) Shanghai Shenhua(8) Beijing Guoan(5) Changchun Yatai(3) Shanghai Port(4) Dalian Pro(15) Tianjin Jinmen Tiger(14) Shanghai Shenhua(8) Beijing Guoan(5) Changchun Yatai(3) Shanghai Port(4) Wuhan FC(12)</t>
-  </si>
-  <si>
-    <t>Henan Songshan Longmen,Shenzhen(6) Cangzhou(13) Shandong Taishan(1) Chongqing Liangjiang Athletic(11) Guangzhou FC(2) Qingdao FC(16) Guangzhou City(9) Shenzhen(6) Cangzhou(13) Shandong Taishan(1) Chongqing Liangjiang Athletic(11) Guangzhou FC(2) Qingdao FC(16) Guangzhou City(9)</t>
-  </si>
-  <si>
-    <t>Qingdao FC,Cangzhou(13) Shenzhen(6) Guangzhou City(9) Shandong Taishan(1) Chongqing Liangjiang Athletic(11) Henan Songshan Longmen(10) Guangzhou FC(2) Cangzhou(13) Shenzhen(6) Guangzhou City(9) Shandong Taishan(1) Chongqing Liangjiang Athletic(11) Henan Songshan Longmen(10) Guangzhou FC(2)</t>
-  </si>
-  <si>
-    <t>Shandong Taishan,Chongqing Liangjiang Athletic(11) Guangzhou FC(2) Henan Songshan Longmen(10) Qingdao FC(16) Shenzhen(6) Guangzhou City(9) Cangzhou(13) Chongqing Liangjiang Athletic(11) Guangzhou FC(2) Henan Songshan Longmen(10) Qingdao FC(16) Shenzhen(6) Guangzhou City(9) Cangzhou(13)</t>
-  </si>
-  <si>
-    <t>Shanghai Port,Tianjin Jinmen Tiger(14) Beijing Guoan(5) Shanghai Shenhua(8) Changchun Yatai(3) Dalian Pro(15) Wuhan FC(12) Hebei(7) Beijing Guoan(5) Shanghai Shenhua(8) Changchun Yatai(3) Dalian Pro(15) Wuhan FC(12) Hebei(7) Tianjin Jinmen Tiger(14)</t>
-  </si>
-  <si>
-    <t>Shanghai Shenhua,Beijing Guoan(5) Wuhan FC(12) Shanghai Port(4) Hebei(7) Changchun Yatai(3) Dalian Pro(15) Tianjin Jinmen Tiger(14) Wuhan FC(12) Shanghai Port(4) Hebei(7) Changchun Yatai(3) Dalian Pro(15) Tianjin Jinmen Tiger(14) Beijing Guoan(5)</t>
-  </si>
-  <si>
-    <t>Shenzhen,Henan Songshan Longmen(10) Qingdao FC(16) Guangzhou FC(2) Guangzhou City(9) Shandong Taishan(1) Cangzhou(13) Chongqing Liangjiang Athletic(11) Henan Songshan Longmen(10) Qingdao FC(16) Guangzhou FC(2) Guangzhou City(9) Shandong Taishan(1) Cangzhou(13) Chongqing Liangjiang Athletic(11)</t>
-  </si>
-  <si>
-    <t>Tianjin Jinmen Tiger,Shanghai Port(4) Changchun Yatai(3) Hebei(7) Dalian Pro(15) Wuhan FC(12) Beijing Guoan(5) Shanghai Shenhua(8) Changchun Yatai(3) Hebei(7) Dalian Pro(15) Wuhan FC(12) Beijing Guoan(5) Shanghai Shenhua(8) Shanghai Port(4)</t>
-  </si>
-  <si>
-    <t>Wuhan FC,Hebei(7) Shanghai Shenhua(8) Changchun Yatai(3) Beijing Guoan(5) Tianjin Jinmen Tiger(14) Shanghai Port(4) Dalian Pro(15) Shanghai Shenhua(8) Changchun Yatai(3) Beijing Guoan(5) Tianjin Jinmen Tiger(14) Shanghai Port(4) Dalian Pro(15) Hebei(7)</t>
+    <t>Beijing Guoan,W W D L W W</t>
+  </si>
+  <si>
+    <t>Cangzhou,L D L L W L</t>
+  </si>
+  <si>
+    <t>Changchun Yatai,D W W W L W</t>
+  </si>
+  <si>
+    <t>Chongqing Liangjiang Athletic,W D L W L L</t>
+  </si>
+  <si>
+    <t>Dalian Pro,L W L L L L</t>
+  </si>
+  <si>
+    <t>Guangzhou City,L W W W L D</t>
+  </si>
+  <si>
+    <t>Guangzhou FC,W L W W W W</t>
+  </si>
+  <si>
+    <t>Hebei,W D D L W D</t>
+  </si>
+  <si>
+    <t>Henan Songshan Longmen,W L W L W D</t>
+  </si>
+  <si>
+    <t>Qingdao FC,L L L L L L</t>
+  </si>
+  <si>
+    <t>Shandong Taishan,L W W W W W</t>
+  </si>
+  <si>
+    <t>Shanghai Port,W L W W L W</t>
+  </si>
+  <si>
+    <t>Shanghai Shenhua,L D L W W L</t>
+  </si>
+  <si>
+    <t>Shenzhen,W W L L L W</t>
+  </si>
+  <si>
+    <t>Tianjin Jinmen Tiger,L L D W L L</t>
+  </si>
+  <si>
+    <t>Wuhan FC,D L D L W D</t>
+  </si>
+  <si>
+    <t>Beijing Guoan,1 2 0 1 2 4,(10)</t>
+  </si>
+  <si>
+    <t>Cangzhou,1 1 2 0 2 1,(7)</t>
+  </si>
+  <si>
+    <t>Changchun Yatai,2 2 2 3 1 3,(13)</t>
+  </si>
+  <si>
+    <t>Chongqing Liangjiang Athletic,4 1 0 1 1 1,(8)</t>
+  </si>
+  <si>
+    <t>Dalian Pro,0 3 0 2 1 1,(7)</t>
+  </si>
+  <si>
+    <t>Guangzhou City,0 4 1 2 1 1,(9)</t>
+  </si>
+  <si>
+    <t>Guangzhou FC,2 1 5 2 5 5,(20)</t>
+  </si>
+  <si>
+    <t>Hebei,2 0 0 0 1 1,(4)</t>
+  </si>
+  <si>
+    <t>Henan Songshan Longmen,2 0 1 0 1 1,(5)</t>
+  </si>
+  <si>
+    <t>Qingdao FC,1 2 0 0 0 0,(3)</t>
+  </si>
+  <si>
+    <t>Shandong Taishan,1 2 5 4 3 2,(17)</t>
+  </si>
+  <si>
+    <t>Shanghai Port,1 1 5 3 0 5,(15)</t>
+  </si>
+  <si>
+    <t>Shanghai Shenhua,0 0 1 4 1 2,(8)</t>
+  </si>
+  <si>
+    <t>Shenzhen,4 2 0 2 1 2,(11)</t>
+  </si>
+  <si>
+    <t>Tianjin Jinmen Tiger,1 1 1 3 0 0,(6)</t>
+  </si>
+  <si>
+    <t>Wuhan FC,2 1 1 0 2 1,(7)</t>
+  </si>
+  <si>
+    <t>Beijing Guoan,0 1 0 3 1 2,(7)</t>
+  </si>
+  <si>
+    <t>Cangzhou,2 1 5 2 1 2,(13)</t>
+  </si>
+  <si>
+    <t>Changchun Yatai,2 1 1 0 2 1,(7)</t>
+  </si>
+  <si>
+    <t>Chongqing Liangjiang Athletic,0 1 1 0 5 2,(9)</t>
+  </si>
+  <si>
+    <t>Dalian Pro,1 1 5 4 2 3,(16)</t>
+  </si>
+  <si>
+    <t>Guangzhou City,4 2 0 0 3 1,(10)</t>
+  </si>
+  <si>
+    <t>Guangzhou FC,1 2 2 0 1 0,(6)</t>
+  </si>
+  <si>
+    <t>Hebei,1 0 0 3 0 1,(5)</t>
+  </si>
+  <si>
+    <t>Henan Songshan Longmen,1 2 0 2 0 1,(6)</t>
+  </si>
+  <si>
+    <t>Qingdao FC,4 4 5 1 1 5,(20)</t>
+  </si>
+  <si>
+    <t>Shandong Taishan,2 0 0 2 1 1,(6)</t>
+  </si>
+  <si>
+    <t>Shanghai Port,0 2 0 0 1 0,(3)</t>
+  </si>
+  <si>
+    <t>Shanghai Shenhua,1 0 2 2 0 4,(9)</t>
+  </si>
+  <si>
+    <t>Shenzhen,1 1 1 4 2 1,(10)</t>
+  </si>
+  <si>
+    <t>Tianjin Jinmen Tiger,2 3 1 1 1 5,(13)</t>
+  </si>
+  <si>
+    <t>Wuhan FC,2 2 1 3 1 1,(10)</t>
+  </si>
+  <si>
+    <t>Beijing Guoan,1 3 0 4 3 6,(17)</t>
+  </si>
+  <si>
+    <t>Cangzhou,3 2 7 2 3 3,(20)</t>
+  </si>
+  <si>
+    <t>Changchun Yatai,4 3 3 3 3 4,(20)</t>
+  </si>
+  <si>
+    <t>Chongqing Liangjiang Athletic,4 2 1 1 6 3,(17)</t>
+  </si>
+  <si>
+    <t>Dalian Pro,1 4 5 6 3 4,(23)</t>
+  </si>
+  <si>
+    <t>Guangzhou City,4 6 1 2 4 2,(19)</t>
+  </si>
+  <si>
+    <t>Guangzhou FC,3 3 7 2 6 5,(26)</t>
+  </si>
+  <si>
+    <t>Hebei,3 0 0 3 1 2,(9)</t>
+  </si>
+  <si>
+    <t>Henan Songshan Longmen,3 2 1 2 1 2,(11)</t>
+  </si>
+  <si>
+    <t>Qingdao FC,5 6 5 1 1 5,(23)</t>
+  </si>
+  <si>
+    <t>Shandong Taishan,3 2 5 6 4 3,(23)</t>
+  </si>
+  <si>
+    <t>Shanghai Port,1 3 5 3 1 5,(18)</t>
+  </si>
+  <si>
+    <t>Shanghai Shenhua,1 0 3 6 1 6,(17)</t>
+  </si>
+  <si>
+    <t>Shenzhen,5 3 1 6 3 3,(21)</t>
+  </si>
+  <si>
+    <t>Tianjin Jinmen Tiger,3 4 2 4 1 5,(19)</t>
+  </si>
+  <si>
+    <t>Wuhan FC,4 3 2 3 3 2,(17)</t>
+  </si>
+  <si>
+    <t>Beijing Guoan,0-1 2-1 0-0 3-1 2-1 4-2</t>
+  </si>
+  <si>
+    <t>Cangzhou,2-1 1-1 5-2 0-2 2-1 2-1</t>
+  </si>
+  <si>
+    <t>Changchun Yatai,2-2 2-1 1-2 3-0 2-1 3-1</t>
+  </si>
+  <si>
+    <t>Chongqing Liangjiang Athletic,4-0 1-1 1-0 1-0 1-5 2-1</t>
+  </si>
+  <si>
+    <t>Dalian Pro,0-1 1-3 0-5 2-4 2-1 3-1</t>
+  </si>
+  <si>
+    <t>Guangzhou City,4-0 4-2 0-1 0-2 1-3 1-1</t>
+  </si>
+  <si>
+    <t>Guangzhou FC,2-1 2-1 5-2 2-0 1-5 5-0</t>
+  </si>
+  <si>
+    <t>Hebei,2-1 0-0 0-0 3-0 1-0 1-1</t>
+  </si>
+  <si>
+    <t>Henan Songshan Longmen,2-1 2-0 1-0 2-0 0-1 1-1</t>
+  </si>
+  <si>
+    <t>Qingdao FC,1-4 4-2 0-5 1-0 0-1 5-0</t>
+  </si>
+  <si>
+    <t>Shandong Taishan,2-1 2-0 0-5 4-2 1-3 2-1</t>
+  </si>
+  <si>
+    <t>Shanghai Port,1-0 2-1 0-5 3-0 1-0 5-0</t>
+  </si>
+  <si>
+    <t>Shanghai Shenhua,1-0 0-0 1-2 2-4 1-0 4-2</t>
+  </si>
+  <si>
+    <t>Shenzhen,1-4 2-1 0-1 4-2 2-1 2-1</t>
+  </si>
+  <si>
+    <t>Tianjin Jinmen Tiger,2-1 1-3 1-1 3-1 1-0 5-0</t>
+  </si>
+  <si>
+    <t>Wuhan FC,2-2 2-1 1-1 3-0 2-1 1-1</t>
+  </si>
+  <si>
+    <t>Beijing Guoan,1 1 0 -2 1 2,(3)</t>
+  </si>
+  <si>
+    <t>Cangzhou,-1 0 -3 -2 1 -1,(-6)</t>
+  </si>
+  <si>
+    <t>Changchun Yatai,0 1 1 3 -1 2,(6)</t>
+  </si>
+  <si>
+    <t>Chongqing Liangjiang Athletic,4 0 -1 1 -4 -1,(-1)</t>
+  </si>
+  <si>
+    <t>Dalian Pro,-1 2 -5 -2 -1 -2,(-9)</t>
+  </si>
+  <si>
+    <t>Guangzhou City,-4 2 1 2 -2 0,(-1)</t>
+  </si>
+  <si>
+    <t>Guangzhou FC,1 -1 3 2 4 5,(14)</t>
+  </si>
+  <si>
+    <t>Hebei,1 0 0 -3 1 0,(-1)</t>
+  </si>
+  <si>
+    <t>Henan Songshan Longmen,1 -2 1 -2 1 0,(-1)</t>
+  </si>
+  <si>
+    <t>Qingdao FC,-3 -2 -5 -1 -1 -5,(-17)</t>
+  </si>
+  <si>
+    <t>Shandong Taishan,-1 2 5 2 2 1,(11)</t>
+  </si>
+  <si>
+    <t>Shanghai Port,1 -1 5 3 -1 5,(12)</t>
+  </si>
+  <si>
+    <t>Shanghai Shenhua,-1 0 -1 2 1 -2,(-1)</t>
+  </si>
+  <si>
+    <t>Shenzhen,3 1 -1 -2 -1 1,(1)</t>
+  </si>
+  <si>
+    <t>Tianjin Jinmen Tiger,-1 -2 0 2 -1 -5,(-7)</t>
+  </si>
+  <si>
+    <t>Wuhan FC,0 -1 0 -3 1 0,(-3)</t>
+  </si>
+  <si>
+    <t>Beijing Guoan,Dalian Pro(15) Wuhan FC(12) Hebei(7) Tianjin Jinmen Tiger(14) Changchun Yatai(3) Shanghai Shenhua(8)</t>
+  </si>
+  <si>
+    <t>Cangzhou,Henan Songshan Longmen(10) Chongqing Liangjiang Athletic(11) Guangzhou FC(2) Guangzhou City(9) Shenzhen(6) Shandong Taishan(1)</t>
+  </si>
+  <si>
+    <t>Changchun Yatai,Wuhan FC(12) Shanghai Port(4) Shanghai Shenhua(8) Hebei(7) Beijing Guoan(5) Dalian Pro(15)</t>
+  </si>
+  <si>
+    <t>Chongqing Liangjiang Athletic,Guangzhou City(9) Cangzhou(13) Henan Songshan Longmen(10) Qingdao FC(16) Guangzhou FC(2) Shenzhen(6)</t>
+  </si>
+  <si>
+    <t>Dalian Pro,Beijing Guoan(5) Tianjin Jinmen Tiger(14) Shanghai Port(4) Shanghai Shenhua(8) Wuhan FC(12) Changchun Yatai(3)</t>
+  </si>
+  <si>
+    <t>Guangzhou City,Chongqing Liangjiang Athletic(11) Qingdao FC(16) Shenzhen(6) Cangzhou(13) Shandong Taishan(1) Henan Songshan Longmen(10)</t>
+  </si>
+  <si>
+    <t>Guangzhou FC,Shandong Taishan(1) Shenzhen(6) Cangzhou(13) Henan Songshan Longmen(10) Chongqing Liangjiang Athletic(11) Qingdao FC(16)</t>
+  </si>
+  <si>
+    <t>Hebei,Tianjin Jinmen Tiger(14) Shanghai Shenhua(8) Beijing Guoan(5) Changchun Yatai(3) Shanghai Port(4) Wuhan FC(12)</t>
+  </si>
+  <si>
+    <t>Henan Songshan Longmen,Cangzhou(13) Shandong Taishan(1) Chongqing Liangjiang Athletic(11) Guangzhou FC(2) Qingdao FC(16) Guangzhou City(9)</t>
+  </si>
+  <si>
+    <t>Qingdao FC,Shenzhen(6) Guangzhou City(9) Shandong Taishan(1) Chongqing Liangjiang Athletic(11) Henan Songshan Longmen(10) Guangzhou FC(2)</t>
+  </si>
+  <si>
+    <t>Shandong Taishan,Guangzhou FC(2) Henan Songshan Longmen(10) Qingdao FC(16) Shenzhen(6) Guangzhou City(9) Cangzhou(13)</t>
+  </si>
+  <si>
+    <t>Shanghai Port,Shanghai Shenhua(8) Changchun Yatai(3) Dalian Pro(15) Wuhan FC(12) Hebei(7) Tianjin Jinmen Tiger(14)</t>
+  </si>
+  <si>
+    <t>Shanghai Shenhua,Shanghai Port(4) Hebei(7) Changchun Yatai(3) Dalian Pro(15) Tianjin Jinmen Tiger(14) Beijing Guoan(5)</t>
+  </si>
+  <si>
+    <t>Shenzhen,Qingdao FC(16) Guangzhou FC(2) Guangzhou City(9) Shandong Taishan(1) Cangzhou(13) Chongqing Liangjiang Athletic(11)</t>
+  </si>
+  <si>
+    <t>Tianjin Jinmen Tiger,Hebei(7) Dalian Pro(15) Wuhan FC(12) Beijing Guoan(5) Shanghai Shenhua(8) Shanghai Port(4)</t>
+  </si>
+  <si>
+    <t>Wuhan FC,Changchun Yatai(3) Beijing Guoan(5) Tianjin Jinmen Tiger(14) Shanghai Port(4) Dalian Pro(15) Hebei(7)</t>
   </si>
   <si>
     <t>chn_division</t>

</xml_diff>